<commit_message>
pembaruan terakhir minus video
</commit_message>
<xml_diff>
--- a/codebook-kamusdata.xlsx
+++ b/codebook-kamusdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Drive\Invited Talks &amp; Workshops\mg-sem-workshop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C6A28FE-7443-4043-ACCE-F68DDDDFDD70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10695BAF-906A-40C6-8E9A-991396EB6630}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="codebook-kamusdata" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="186">
   <si>
     <t>Nama Variabel</t>
   </si>
@@ -584,6 +584,10 @@
   </si>
   <si>
     <t>Termometer sikap: Prabowo</t>
+  </si>
+  <si>
+    <t>1: Sangat TIDAK SEJALAN dengan pendapat saya
+7: Sangat SEJALAN dengan pendapat saya</t>
   </si>
 </sst>
 </file>
@@ -1472,7 +1476,7 @@
   <dimension ref="A1:D87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1519,7 +1523,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>10</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">

</xml_diff>